<commit_message>
updated verify added client
</commit_message>
<xml_diff>
--- a/ProjectServiceManagement/src/main/java/Resources/testdata.xlsx
+++ b/ProjectServiceManagement/src/main/java/Resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanda\git\ServiceManagement_Project\ProjectServiceManagement\src\main\java\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E610006-0B2C-4663-9901-68A12E87615E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA3E8B9-08C6-4F0D-8403-0B4858095CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="139" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="0" windowWidth="17496" windowHeight="12240" tabRatio="139" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testSheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Username</t>
   </si>
@@ -310,10 +310,16 @@
     <t>Reparation_AddServiceCharge</t>
   </si>
   <si>
-    <t>Aron</t>
-  </si>
-  <si>
     <t>Add_Reparation expected message</t>
+  </si>
+  <si>
+    <t>Ajim</t>
+  </si>
+  <si>
+    <t>Add_Client Message</t>
+  </si>
+  <si>
+    <t>Client: Ajim</t>
   </si>
 </sst>
 </file>
@@ -661,7 +667,7 @@
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
@@ -1024,12 +1030,18 @@
     </row>
     <row r="7" spans="1:35" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>